<commit_message>
Update excel and index.html
</commit_message>
<xml_diff>
--- a/DSNY_and_NonDSNY_Collections_by_Fiscal_Year.xlsx
+++ b/DSNY_and_NonDSNY_Collections_by_Fiscal_Year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jui/Documents/Columbia_Academics_2021_22/Spring_2022/Data_Studio/Project_2/project_2_analysis/nyc-recycling-distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4392428E-5E6D-B74E-99C1-D9AB2E2E8BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5005DF89-ECFB-1442-AB46-1024310DB53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30500" yWindow="-3100" windowWidth="35360" windowHeight="20100" xr2:uid="{E5D9DE3E-A9EA-9944-8F3A-485463A2893F}"/>
   </bookViews>
@@ -294,48 +294,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -710,7 +710,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:P10"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,589 +719,589 @@
     <col min="5" max="5" width="60.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" ht="31" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:16" ht="11" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
     </row>
     <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="14" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
     </row>
     <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="9" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="9" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="8" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="8" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="8" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="8" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="8" t="s">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="13" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="20"/>
+      <c r="P30" s="20"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="7"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1310,6 +1310,38 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A1:E4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D14:P15"/>
+    <mergeCell ref="A10:P10"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D12:P12"/>
+    <mergeCell ref="D13:P13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D11:P11"/>
+    <mergeCell ref="D19:P19"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D28:P28"/>
+    <mergeCell ref="D29:P29"/>
+    <mergeCell ref="A31:P31"/>
+    <mergeCell ref="A18:P18"/>
+    <mergeCell ref="D21:P21"/>
+    <mergeCell ref="D20:P20"/>
+    <mergeCell ref="D30:P30"/>
+    <mergeCell ref="D22:P22"/>
+    <mergeCell ref="D26:P26"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="D6:P9"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D23:P23"/>
@@ -1322,40 +1354,8 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:P16"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D28:P28"/>
-    <mergeCell ref="D29:P29"/>
-    <mergeCell ref="A31:P31"/>
-    <mergeCell ref="A18:P18"/>
-    <mergeCell ref="D21:P21"/>
-    <mergeCell ref="D20:P20"/>
-    <mergeCell ref="D30:P30"/>
-    <mergeCell ref="D22:P22"/>
-    <mergeCell ref="D26:P26"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D14:P15"/>
-    <mergeCell ref="A10:P10"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D12:P12"/>
-    <mergeCell ref="D13:P13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D11:P11"/>
-    <mergeCell ref="D19:P19"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A1:E4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:E4" r:id="rId1" display="https://dsny.cityofnewyork.us/wp-content/uploads/2017/12/about_dsny-non-dsny-collections-FY2011_0815.pdf" xr:uid="{207D1680-E75F-0C4A-BCA5-96A2045830C4}"/>
@@ -1423,7 +1423,7 @@
       <c r="H1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1461,705 +1461,705 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="A2" s="5">
         <v>2011</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="4">
         <v>1062</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="4">
         <v>714</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="4">
         <v>0.5</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="4">
         <v>8.6</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="4">
         <v>0.72</v>
       </c>
-      <c r="I2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="15">
+      <c r="I2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="4">
         <v>38.33</v>
       </c>
-      <c r="L2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="15">
+      <c r="L2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="4">
         <v>7.84</v>
       </c>
-      <c r="O2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="15">
+      <c r="O2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="4">
         <v>1.94</v>
       </c>
-      <c r="Q2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="15">
+      <c r="Q2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4">
         <v>0.2</v>
       </c>
-      <c r="S2" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="23" t="s">
+      <c r="S2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="5">
         <v>2012</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="4">
         <v>1028</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="4">
         <v>706</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="4">
         <v>4</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="15">
+      <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4">
         <v>10.83</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="4">
         <v>5.88</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="4">
         <v>2.0499999999999998</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4">
         <v>177</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="4">
         <v>117</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="4">
         <v>0.67</v>
       </c>
-      <c r="M3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="15">
+      <c r="M3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="4">
         <v>3.29</v>
       </c>
-      <c r="O3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="15">
+      <c r="O3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" s="4">
         <v>6.45</v>
       </c>
-      <c r="Q3" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="15">
+      <c r="Q3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="4">
         <v>4.54</v>
       </c>
-      <c r="S3" s="15">
+      <c r="S3" s="4">
         <v>0.1</v>
       </c>
-      <c r="T3" s="23" t="s">
+      <c r="T3" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="5">
         <v>2013</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="4">
         <v>1015</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="4">
         <v>699</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4">
         <v>17</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="4">
         <v>6</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="4">
         <v>1.6</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="I4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4">
         <v>176.5</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="4">
         <v>85.7</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="M4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="15">
+      <c r="M4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" s="4">
         <v>21.3</v>
       </c>
-      <c r="O4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="15">
+      <c r="O4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="4">
         <v>17.399999999999999</v>
       </c>
-      <c r="Q4" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="15">
+      <c r="Q4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="4">
         <v>7.2</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="4">
         <v>0.1</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="T4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+      <c r="A5" s="5">
         <v>2014</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="4">
         <v>1007</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="4">
         <v>748</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="4">
         <v>19</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="E5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4">
         <v>38</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="4">
         <v>6</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="I5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="4">
         <v>173</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="4">
         <v>62</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="4">
         <v>5</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="4">
         <v>2</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="4">
         <v>11</v>
       </c>
-      <c r="O5" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="15">
+      <c r="O5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="4">
         <v>6</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="4">
         <v>0.2</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="4">
         <v>8</v>
       </c>
-      <c r="S5" s="15">
+      <c r="S5" s="4">
         <v>0.1</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="T5" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="5">
         <v>2015</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="4">
         <v>1018</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="4">
         <v>784</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="4">
         <v>43</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="E6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4">
         <v>42</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="4">
         <v>5</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="4">
         <v>2</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="4">
         <v>174</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="4">
         <v>56</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="4">
         <v>5</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="4">
         <v>4</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="4">
         <v>20</v>
       </c>
-      <c r="O6" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P6" s="15">
+      <c r="O6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="4">
         <v>31</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="4">
         <v>1</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="4">
         <v>13</v>
       </c>
-      <c r="S6" s="15">
+      <c r="S6" s="4">
         <v>0</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="T6" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
+      <c r="A7" s="5">
         <v>2016</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="4">
         <v>1045.0999999999999</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>863</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="4">
         <v>59.2</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="15">
+      <c r="E7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4">
         <v>49.4</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="4">
         <v>4.7</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="4">
         <v>2.8</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="4">
         <v>0.2</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="4">
         <v>195.4</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="4">
         <v>59.1</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="4">
         <v>5.7</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="4">
         <v>30.8</v>
       </c>
-      <c r="O7" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="15">
+      <c r="O7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="4">
         <v>33.4</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="4">
         <v>7.2</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="4">
         <v>11.4</v>
       </c>
-      <c r="S7" s="15">
+      <c r="S7" s="4">
         <v>0.1</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="T7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="5">
         <v>2017</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="4">
         <v>1056</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="4">
         <v>917.4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="4">
         <v>81.400000000000006</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="E8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4">
         <v>54.2</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="4">
         <v>2.4</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="4">
         <v>0.3</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="4">
         <v>208.7</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="4">
         <v>69.7</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="4">
         <v>5.5</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="4">
         <v>5.4</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="4">
         <v>41.4</v>
       </c>
-      <c r="O8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="P8" s="15">
+      <c r="O8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="4">
         <v>93.7</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="4">
         <v>8.6</v>
       </c>
-      <c r="R8" s="15">
+      <c r="R8" s="4">
         <v>14.2</v>
       </c>
-      <c r="S8" s="15">
+      <c r="S8" s="4">
         <v>0.1</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="T8" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="5">
         <v>2018</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="4">
         <v>1043</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="4">
         <v>934.7</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="4">
         <v>141</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="4">
         <v>46.7</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="4">
         <v>4.8</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="4">
         <v>3</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="4">
         <v>0.1</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="4">
         <v>209.7</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="4">
         <v>82.6</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="4">
         <v>6.6</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="4">
         <v>6.1</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="4">
         <v>53.9</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="4">
         <v>100.9</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="4">
         <v>25.7</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="Q9" s="4">
         <v>9.6</v>
       </c>
-      <c r="R9" s="15">
+      <c r="R9" s="4">
         <v>7.4</v>
       </c>
-      <c r="S9" s="15">
+      <c r="S9" s="4">
         <v>0.1</v>
       </c>
-      <c r="T9" s="23" t="s">
+      <c r="T9" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="5">
         <v>2019</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="4">
         <v>1061.5</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="4">
         <v>964.6</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="4">
         <v>154.30000000000001</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="4">
         <v>46.6</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="4">
         <v>5.5</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="4">
         <v>2.8</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="4">
         <v>0.4</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="4">
         <v>231.5</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="4">
         <v>79.900000000000006</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="4">
         <v>8.1</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="4">
         <v>7.4</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="4">
         <v>45.7</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="4">
         <v>104.4</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="4">
         <v>24.2</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="Q10" s="4">
         <v>9.4</v>
       </c>
-      <c r="R10" s="15">
+      <c r="R10" s="4">
         <v>18.7</v>
       </c>
-      <c r="S10" s="15">
+      <c r="S10" s="4">
         <v>0.1</v>
       </c>
-      <c r="T10" s="23" t="s">
+      <c r="T10" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="5">
         <v>2020</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="4">
         <v>1033</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="4">
         <v>1038.8</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="4">
         <v>123.4</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="4">
         <v>0</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="4">
         <v>43</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="4">
         <v>6.5</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="4">
         <v>2</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="4">
         <v>0.3</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="4">
         <v>240.9</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="4">
         <v>75.099999999999994</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="4">
         <v>6.7</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="4">
         <v>5.2</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="4">
         <v>37</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="4">
         <v>142.19999999999999</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="4">
         <v>17.3</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="4">
         <v>7.8</v>
       </c>
-      <c r="R11" s="15">
+      <c r="R11" s="4">
         <v>22.8</v>
       </c>
-      <c r="S11" s="15">
+      <c r="S11" s="4">
         <v>0.1</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="T11" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="5">
         <v>2021</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="4">
         <v>1087.3</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="4">
         <v>1110.3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="4">
         <v>6.6</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="7">
         <v>36.1</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="7">
         <v>6.5</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="7">
         <v>0.1</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="7">
         <v>0.1</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="4">
         <v>229.9</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="4">
         <v>82.2</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="4">
         <v>6.3</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="4">
         <v>33.200000000000003</v>
       </c>
-      <c r="O12" s="15">
+      <c r="O12" s="4">
         <v>227.2</v>
       </c>
-      <c r="P12" s="15">
+      <c r="P12" s="4">
         <v>10.9</v>
       </c>
-      <c r="Q12" s="15">
+      <c r="Q12" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R12" s="15">
+      <c r="R12" s="4">
         <v>24.4</v>
       </c>
-      <c r="S12" s="15">
+      <c r="S12" s="4">
         <v>0.1</v>
       </c>
-      <c r="T12" s="23" t="s">
+      <c r="T12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="E13" s="22"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D14" s="15"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D15" s="15"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D16" s="15"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="15"/>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2191,156 +2191,156 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="A2" s="5">
         <v>2011</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="4">
         <v>1062</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="4">
         <v>714</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="5">
         <v>2012</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="4">
         <v>1028</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="4">
         <v>706</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="5">
         <v>2013</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="4">
         <v>1015</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="4">
         <v>699</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="4">
         <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+      <c r="A5" s="5">
         <v>2014</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="4">
         <v>1007</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="4">
         <v>748</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="4">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
+      <c r="A6" s="5">
         <v>2015</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="4">
         <v>1018</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="4">
         <v>784</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="4">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
+      <c r="A7" s="5">
         <v>2016</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="4">
         <v>1045.0999999999999</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="4">
         <v>863</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="4">
         <v>59.2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
+      <c r="A8" s="5">
         <v>2017</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="4">
         <v>1056</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="4">
         <v>917.4</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="4">
         <v>81.400000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="16">
+      <c r="A9" s="5">
         <v>2018</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="4">
         <v>1043</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="4">
         <v>934.7</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="4">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="16">
+      <c r="A10" s="5">
         <v>2019</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="4">
         <v>1061.5</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="4">
         <v>964.6</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="4">
         <v>154.30000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="16">
+      <c r="A11" s="5">
         <v>2020</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="4">
         <v>1033</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="4">
         <v>1038.8</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="4">
         <v>123.4</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="16">
+      <c r="A12" s="5">
         <v>2021</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="4">
         <v>1087.3</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="4">
         <v>1110.3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="4">
         <v>6.6</v>
       </c>
     </row>
@@ -2352,7 +2352,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="21"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2365,24 +2365,24 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2396,7 +2396,7 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="4">
         <v>1087.3</v>
       </c>
     </row>
@@ -2404,7 +2404,7 @@
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="4">
         <v>1110.3</v>
       </c>
     </row>
@@ -2412,7 +2412,7 @@
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="4">
         <v>6.6</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="7">
         <v>36.1</v>
       </c>
     </row>
@@ -2428,7 +2428,7 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="7">
         <v>6.5</v>
       </c>
     </row>
@@ -2436,15 +2436,15 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B24" s="7">
         <v>0.1</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="7">
         <v>0.1</v>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="15">
+      <c r="B26" s="4">
         <v>229.9</v>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="15">
+      <c r="B27" s="4">
         <v>82.2</v>
       </c>
     </row>
@@ -2468,7 +2468,7 @@
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="4">
         <v>6.3</v>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B29" s="4">
         <v>4.9000000000000004</v>
       </c>
     </row>
@@ -2484,7 +2484,7 @@
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="15">
+      <c r="B30" s="4">
         <v>33.200000000000003</v>
       </c>
     </row>
@@ -2492,7 +2492,7 @@
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="4">
         <v>227.2</v>
       </c>
     </row>
@@ -2500,7 +2500,7 @@
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="15">
+      <c r="B32" s="4">
         <v>10.9</v>
       </c>
     </row>
@@ -2508,7 +2508,7 @@
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="4">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -2516,7 +2516,7 @@
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="4">
         <v>24.4</v>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="15">
+      <c r="B35" s="4">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>